<commit_message>
metal for approach 4
</commit_message>
<xml_diff>
--- a/dna-methylation/scripts/develop/illumina450k/betas/plot/scatter_comparison_rows.xlsx
+++ b/dna-methylation/scripts/develop/illumina450k/betas/plot/scatter_comparison_rows.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="23">
   <si>
     <t>begins</t>
   </si>
@@ -36,55 +36,58 @@
     <t>auto</t>
   </si>
   <si>
-    <t>cg14348741</t>
-  </si>
-  <si>
-    <t>cg26584545</t>
-  </si>
-  <si>
-    <t>cg01620164</t>
-  </si>
-  <si>
-    <t>cg25282715</t>
+    <t>cg03076319</t>
+  </si>
+  <si>
+    <t>cg10001590</t>
+  </si>
+  <si>
+    <t>cg18157012</t>
+  </si>
+  <si>
+    <t>cg23713156</t>
+  </si>
+  <si>
+    <t>cg12614148</t>
+  </si>
+  <si>
+    <t>SLIT3</t>
+  </si>
+  <si>
+    <t>cg16910042</t>
+  </si>
+  <si>
+    <t>cg08464177</t>
+  </si>
+  <si>
+    <t>BAI1</t>
   </si>
   <si>
     <t>cg15634877</t>
   </si>
   <si>
-    <t>cg21449170</t>
-  </si>
-  <si>
-    <t>cg21529533</t>
-  </si>
-  <si>
-    <t>cg26682094</t>
-  </si>
-  <si>
-    <t>cg04194272</t>
-  </si>
-  <si>
-    <t>cg04832177</t>
-  </si>
-  <si>
-    <t>cg26522743</t>
-  </si>
-  <si>
-    <t>cg17774851</t>
-  </si>
-  <si>
-    <t>cg27143204</t>
-  </si>
-  <si>
-    <t>cg06158650</t>
-  </si>
-  <si>
-    <t>cg27537164</t>
-  </si>
-  <si>
-    <t>cg19481686</t>
-  </si>
-  <si>
-    <t>cg07613182</t>
+    <t>cg14030346</t>
+  </si>
+  <si>
+    <t>cg11537828</t>
+  </si>
+  <si>
+    <t>SPEG</t>
+  </si>
+  <si>
+    <t>CNPY1</t>
+  </si>
+  <si>
+    <t>MLPH</t>
+  </si>
+  <si>
+    <t>PTPRN2</t>
+  </si>
+  <si>
+    <t>WDR45L</t>
+  </si>
+  <si>
+    <t>CADM1</t>
   </si>
 </sst>
 </file>
@@ -452,13 +455,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D18"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="20.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="20.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
@@ -476,7 +479,10 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>7</v>
+        <v>8</v>
+      </c>
+      <c r="B2" t="s">
+        <v>21</v>
       </c>
       <c r="C2" t="s">
         <v>4</v>
@@ -487,7 +493,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C3" t="s">
         <v>4</v>
@@ -498,7 +504,10 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>9</v>
+        <v>15</v>
+      </c>
+      <c r="B4" t="s">
+        <v>22</v>
       </c>
       <c r="C4" t="s">
         <v>4</v>
@@ -509,7 +518,10 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>10</v>
+        <v>16</v>
+      </c>
+      <c r="B5" t="s">
+        <v>18</v>
       </c>
       <c r="C5" t="s">
         <v>4</v>
@@ -520,7 +532,10 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>11</v>
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>19</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -531,7 +546,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C7" t="s">
         <v>4</v>
@@ -542,6 +557,9 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" t="s">
         <v>13</v>
       </c>
       <c r="C8" t="s">
@@ -555,6 +573,9 @@
       <c r="A9" t="s">
         <v>14</v>
       </c>
+      <c r="B9" t="s">
+        <v>17</v>
+      </c>
       <c r="C9" t="s">
         <v>4</v>
       </c>
@@ -564,7 +585,10 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>6</v>
+        <v>7</v>
+      </c>
+      <c r="B10" t="s">
+        <v>10</v>
       </c>
       <c r="C10" t="s">
         <v>4</v>
@@ -575,7 +599,10 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>15</v>
+        <v>11</v>
+      </c>
+      <c r="B11" t="s">
+        <v>20</v>
       </c>
       <c r="C11" t="s">
         <v>4</v>
@@ -584,84 +611,10 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>16</v>
-      </c>
-      <c r="C12" t="s">
-        <v>4</v>
-      </c>
-      <c r="D12" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>5</v>
-      </c>
-      <c r="C13" t="s">
-        <v>4</v>
-      </c>
-      <c r="D13" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>17</v>
-      </c>
-      <c r="C14" t="s">
-        <v>4</v>
-      </c>
-      <c r="D14" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>18</v>
-      </c>
-      <c r="C15" t="s">
-        <v>4</v>
-      </c>
-      <c r="D15" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>19</v>
-      </c>
-      <c r="C16" t="s">
-        <v>4</v>
-      </c>
-      <c r="D16" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>20</v>
-      </c>
-      <c r="C17" t="s">
-        <v>4</v>
-      </c>
-      <c r="D17" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>21</v>
-      </c>
-      <c r="C18" t="s">
-        <v>4</v>
-      </c>
-      <c r="D18" t="s">
-        <v>4</v>
-      </c>
-    </row>
   </sheetData>
+  <sortState ref="A30:C44">
+    <sortCondition descending="1" ref="B30:B44"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
common ssaDMPs and ssaVMPs
</commit_message>
<xml_diff>
--- a/dna-methylation/scripts/develop/illumina450k/betas/plot/scatter_comparison_rows.xlsx
+++ b/dna-methylation/scripts/develop/illumina450k/betas/plot/scatter_comparison_rows.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="23">
   <si>
     <t>begins</t>
   </si>
@@ -36,25 +36,34 @@
     <t>auto</t>
   </si>
   <si>
-    <t>cg03076319</t>
-  </si>
-  <si>
-    <t>cg10001590</t>
-  </si>
-  <si>
-    <t>cg18157012</t>
-  </si>
-  <si>
-    <t>cg23713156</t>
-  </si>
-  <si>
-    <t>cg12614148</t>
-  </si>
-  <si>
-    <t>SLIT3</t>
-  </si>
-  <si>
-    <t>cg16910042</t>
+    <t>cg06904667</t>
+  </si>
+  <si>
+    <t>cg04202002</t>
+  </si>
+  <si>
+    <t>cg16786971</t>
+  </si>
+  <si>
+    <t>cg15122985</t>
+  </si>
+  <si>
+    <t>cg14506657</t>
+  </si>
+  <si>
+    <t>cg24482850</t>
+  </si>
+  <si>
+    <t>cg20403557</t>
+  </si>
+  <si>
+    <t>cg10317815</t>
+  </si>
+  <si>
+    <t>cg15634877</t>
+  </si>
+  <si>
+    <t>SPEG</t>
   </si>
   <si>
     <t>cg08464177</t>
@@ -63,31 +72,22 @@
     <t>BAI1</t>
   </si>
   <si>
-    <t>cg15634877</t>
-  </si>
-  <si>
-    <t>cg14030346</t>
-  </si>
-  <si>
-    <t>cg11537828</t>
-  </si>
-  <si>
-    <t>SPEG</t>
-  </si>
-  <si>
-    <t>CNPY1</t>
-  </si>
-  <si>
-    <t>MLPH</t>
-  </si>
-  <si>
-    <t>PTPRN2</t>
-  </si>
-  <si>
-    <t>WDR45L</t>
-  </si>
-  <si>
-    <t>CADM1</t>
+    <t>TCEA2</t>
+  </si>
+  <si>
+    <t>NUAK2</t>
+  </si>
+  <si>
+    <t>LVRN</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t>reverses</t>
   </si>
 </sst>
 </file>
@@ -119,7 +119,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -142,13 +142,27 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -455,15 +469,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="G29" sqref="G29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -476,13 +490,16 @@
       <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E1" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="B2" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="C2" t="s">
         <v>4</v>
@@ -490,10 +507,13 @@
       <c r="D2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="C3" t="s">
         <v>4</v>
@@ -501,13 +521,16 @@
       <c r="D3" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>15</v>
       </c>
       <c r="B4" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="C4" t="s">
         <v>4</v>
@@ -515,13 +538,13 @@
       <c r="D4" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>16</v>
-      </c>
-      <c r="B5" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="C5" t="s">
         <v>4</v>
@@ -529,13 +552,16 @@
       <c r="D5" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="B6" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -543,8 +569,11 @@
       <c r="D6" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>9</v>
       </c>
@@ -554,13 +583,16 @@
       <c r="D7" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B8" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="C8" t="s">
         <v>4</v>
@@ -568,13 +600,16 @@
       <c r="D8" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B9" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C9" t="s">
         <v>4</v>
@@ -582,13 +617,13 @@
       <c r="D9" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E9" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>7</v>
-      </c>
-      <c r="B10" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C10" t="s">
         <v>4</v>
@@ -596,19 +631,22 @@
       <c r="D10" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E10" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>11</v>
-      </c>
-      <c r="B11" t="s">
-        <v>20</v>
+        <v>6</v>
       </c>
       <c r="C11" t="s">
         <v>4</v>
       </c>
       <c r="D11" t="s">
         <v>4</v>
+      </c>
+      <c r="E11" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
approach 3 direction in progress
</commit_message>
<xml_diff>
--- a/dna-methylation/scripts/develop/illumina450k/betas/plot/scatter_comparison_rows.xlsx
+++ b/dna-methylation/scripts/develop/illumina450k/betas/plot/scatter_comparison_rows.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="25">
   <si>
     <t>begins</t>
   </si>
@@ -36,58 +36,64 @@
     <t>auto</t>
   </si>
   <si>
-    <t>cg06904667</t>
-  </si>
-  <si>
-    <t>cg04202002</t>
-  </si>
-  <si>
-    <t>cg16786971</t>
-  </si>
-  <si>
-    <t>cg15122985</t>
-  </si>
-  <si>
-    <t>cg14506657</t>
-  </si>
-  <si>
-    <t>cg24482850</t>
-  </si>
-  <si>
-    <t>cg20403557</t>
-  </si>
-  <si>
-    <t>cg10317815</t>
-  </si>
-  <si>
-    <t>cg15634877</t>
-  </si>
-  <si>
-    <t>SPEG</t>
-  </si>
-  <si>
-    <t>cg08464177</t>
-  </si>
-  <si>
-    <t>BAI1</t>
-  </si>
-  <si>
-    <t>TCEA2</t>
-  </si>
-  <si>
-    <t>NUAK2</t>
-  </si>
-  <si>
-    <t>LVRN</t>
-  </si>
-  <si>
-    <t>yes</t>
-  </si>
-  <si>
     <t>no</t>
   </si>
   <si>
     <t>reverses</t>
+  </si>
+  <si>
+    <t>cg08369368</t>
+  </si>
+  <si>
+    <t>cg03890691</t>
+  </si>
+  <si>
+    <t>cg15772157</t>
+  </si>
+  <si>
+    <t>cg24789467</t>
+  </si>
+  <si>
+    <t>cg02716826</t>
+  </si>
+  <si>
+    <t>cg27151362</t>
+  </si>
+  <si>
+    <t>cg26612727</t>
+  </si>
+  <si>
+    <t>cg23960707</t>
+  </si>
+  <si>
+    <t>cg26276120</t>
+  </si>
+  <si>
+    <t>cg18310639</t>
+  </si>
+  <si>
+    <t>DOC2A</t>
+  </si>
+  <si>
+    <t>SHROOM1</t>
+  </si>
+  <si>
+    <t>SUGT1P1;AQP3</t>
+  </si>
+  <si>
+    <t>NSD1</t>
+  </si>
+  <si>
+    <t>ZPBP2</t>
+  </si>
+  <si>
+    <t>SFRS1</t>
+  </si>
+  <si>
+    <t>TPI1</t>
+  </si>
+  <si>
+    <t>CAPN2</t>
   </si>
 </sst>
 </file>
@@ -472,7 +478,7 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G29" sqref="G29"/>
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -491,15 +497,15 @@
         <v>1</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>22</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="B2" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="C2" t="s">
         <v>4</v>
@@ -508,12 +514,15 @@
         <v>4</v>
       </c>
       <c r="E2" t="s">
-        <v>20</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>12</v>
+        <v>8</v>
+      </c>
+      <c r="B3" t="s">
+        <v>17</v>
       </c>
       <c r="C3" t="s">
         <v>4</v>
@@ -522,15 +531,12 @@
         <v>4</v>
       </c>
       <c r="E3" t="s">
-        <v>20</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>15</v>
-      </c>
-      <c r="B4" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="C4" t="s">
         <v>4</v>
@@ -539,12 +545,15 @@
         <v>4</v>
       </c>
       <c r="E4" t="s">
-        <v>20</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>7</v>
+        <v>10</v>
+      </c>
+      <c r="B5" t="s">
+        <v>18</v>
       </c>
       <c r="C5" t="s">
         <v>4</v>
@@ -553,15 +562,15 @@
         <v>4</v>
       </c>
       <c r="E5" t="s">
-        <v>21</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B6" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -570,12 +579,15 @@
         <v>4</v>
       </c>
       <c r="E6" t="s">
-        <v>21</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>9</v>
+        <v>12</v>
+      </c>
+      <c r="B7" t="s">
+        <v>17</v>
       </c>
       <c r="C7" t="s">
         <v>4</v>
@@ -584,15 +596,15 @@
         <v>4</v>
       </c>
       <c r="E7" t="s">
-        <v>21</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="B8" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="C8" t="s">
         <v>4</v>
@@ -601,15 +613,15 @@
         <v>4</v>
       </c>
       <c r="E8" t="s">
-        <v>21</v>
+        <v>5</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B9" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="C9" t="s">
         <v>4</v>
@@ -618,12 +630,15 @@
         <v>4</v>
       </c>
       <c r="E9" t="s">
-        <v>21</v>
+        <v>5</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>5</v>
+        <v>15</v>
+      </c>
+      <c r="B10" t="s">
+        <v>23</v>
       </c>
       <c r="C10" t="s">
         <v>4</v>
@@ -632,12 +647,15 @@
         <v>4</v>
       </c>
       <c r="E10" t="s">
-        <v>21</v>
+        <v>5</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>6</v>
+        <v>16</v>
+      </c>
+      <c r="B11" t="s">
+        <v>24</v>
       </c>
       <c r="C11" t="s">
         <v>4</v>
@@ -646,7 +664,7 @@
         <v>4</v>
       </c>
       <c r="E11" t="s">
-        <v>21</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>